<commit_message>
redownloaded parliamant files to be in original state to act as an archive
</commit_message>
<xml_diff>
--- a/raw_data/alle_Anfragen_Beantwortungen/Beantwortungen/pdfs/2024-12-20_INR_12_beantwortet_19J/Beilage_2.xlsx
+++ b/raw_data/alle_Anfragen_Beantwortungen/Beantwortungen/pdfs/2024-12-20_INR_12_beantwortet_19J/Beilage_2.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\WU\WARRA\raw_data\alle_Anfragen_Beantwortungen\Beantwortungen\pdfs\2024-12-20_INR_12_beantwortet_19J\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25258AFB-1084-4D12-971D-4A4643775C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22440" yWindow="-16335" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Frage 1" sheetId="2" r:id="rId1"/>
     <sheet name="Frage 2" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Anzahl PAT_SVS</t>
   </si>
@@ -175,28 +169,13 @@
   </si>
   <si>
     <t>Dentist</t>
-  </si>
-  <si>
-    <t>Summe</t>
-  </si>
-  <si>
-    <t>Antragsanzahl aus Parlamentsbeantwortung 18726/AB (nicht für alle Fachgebiete verfügbar)</t>
-  </si>
-  <si>
-    <t>Summe für Fachgebiete wo Daten verfügbar</t>
-  </si>
-  <si>
-    <t>Summe für Fachgebiete wo keine Daten verfügbar</t>
-  </si>
-  <si>
-    <t>Zahnarztanträge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,9 +305,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Standard 7" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 4" xfId="2"/>
+    <cellStyle name="Standard 7" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,14 +638,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.25" style="6"/>
     <col min="2" max="2" width="64" style="5" bestFit="1" customWidth="1"/>
@@ -674,17 +653,17 @@
     <col min="4" max="16384" width="11.25" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="21.2" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="21.2" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -694,11 +673,8 @@
       <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="9">
         <v>1</v>
       </c>
@@ -708,15 +684,8 @@
       <c r="C5" s="10">
         <v>49380</v>
       </c>
-      <c r="F5" s="3">
-        <v>131668</v>
-      </c>
-      <c r="G5" s="3">
-        <f>F5/C5</f>
-        <v>2.6664236533009316</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -726,12 +695,8 @@
       <c r="C6" s="10">
         <v>1629</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" ref="G6:G34" si="0">F6/C6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -741,15 +706,8 @@
       <c r="C7" s="10">
         <v>58224</v>
       </c>
-      <c r="F7" s="3">
-        <v>80808</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="0"/>
-        <v>1.3878812860676011</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -759,15 +717,8 @@
       <c r="C8" s="10">
         <v>14344</v>
       </c>
-      <c r="F8" s="3">
-        <v>20518</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.4304238706079198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="9">
         <v>5</v>
       </c>
@@ -777,15 +728,8 @@
       <c r="C9" s="10">
         <v>55406</v>
       </c>
-      <c r="F9" s="3">
-        <v>80035</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="0"/>
-        <v>1.4445186441901599</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -795,15 +739,8 @@
       <c r="C10" s="10">
         <v>57199</v>
       </c>
-      <c r="F10" s="3">
-        <v>87008</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5211454745712338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -813,12 +750,8 @@
       <c r="C11" s="10">
         <v>53890</v>
       </c>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -828,15 +761,8 @@
       <c r="C12" s="10">
         <v>17790</v>
       </c>
-      <c r="F12" s="3">
-        <v>51537</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="0"/>
-        <v>2.896964586846543</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="9">
         <v>9</v>
       </c>
@@ -846,12 +772,8 @@
       <c r="C13" s="10">
         <v>19632</v>
       </c>
-      <c r="G13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -861,12 +783,8 @@
       <c r="C14" s="10">
         <v>4002</v>
       </c>
-      <c r="G14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -876,12 +794,8 @@
       <c r="C15" s="10">
         <v>2978</v>
       </c>
-      <c r="G15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -891,15 +805,8 @@
       <c r="C16" s="10">
         <v>38280</v>
       </c>
-      <c r="F16" s="3">
-        <v>77611</v>
-      </c>
-      <c r="G16" s="3">
-        <f t="shared" si="0"/>
-        <v>2.0274555903866247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -909,12 +816,8 @@
       <c r="C17" s="10">
         <v>2737</v>
       </c>
-      <c r="G17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -924,12 +827,8 @@
       <c r="C18" s="10">
         <v>6167</v>
       </c>
-      <c r="G18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="9">
         <v>15</v>
       </c>
@@ -939,12 +838,8 @@
       <c r="C19" s="10">
         <v>11669</v>
       </c>
-      <c r="G19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="9">
         <v>16</v>
       </c>
@@ -954,15 +849,8 @@
       <c r="C20" s="10">
         <v>21537</v>
       </c>
-      <c r="F20" s="3">
-        <v>32213</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="0"/>
-        <v>1.4957050657008868</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="9">
         <v>17</v>
       </c>
@@ -972,12 +860,8 @@
       <c r="C21" s="10">
         <v>104484</v>
       </c>
-      <c r="G21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="9">
         <v>18</v>
       </c>
@@ -987,12 +871,8 @@
       <c r="C22" s="10">
         <v>2573</v>
       </c>
-      <c r="G22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="9">
         <v>19</v>
       </c>
@@ -1002,12 +882,8 @@
       <c r="C23" s="10">
         <v>10249</v>
       </c>
-      <c r="G23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="9">
         <v>20</v>
       </c>
@@ -1017,15 +893,8 @@
       <c r="C24" s="10">
         <v>6670</v>
       </c>
-      <c r="F24" s="3">
-        <v>23418</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" si="0"/>
-        <v>3.510944527736132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="9">
         <v>21</v>
       </c>
@@ -1035,12 +904,8 @@
       <c r="C25" s="10">
         <v>1658</v>
       </c>
-      <c r="G25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="9">
         <v>22</v>
       </c>
@@ -1050,12 +915,8 @@
       <c r="C26" s="10">
         <v>302</v>
       </c>
-      <c r="G26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="9">
         <v>23</v>
       </c>
@@ -1065,12 +926,8 @@
       <c r="C27" s="10">
         <v>1120</v>
       </c>
-      <c r="G27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="9">
         <v>24</v>
       </c>
@@ -1080,12 +937,8 @@
       <c r="C28" s="10">
         <v>4041</v>
       </c>
-      <c r="G28" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -1095,12 +948,8 @@
       <c r="C29" s="10">
         <v>114</v>
       </c>
-      <c r="G29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -1110,12 +959,8 @@
       <c r="C30" s="10">
         <v>68082</v>
       </c>
-      <c r="G30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -1125,12 +970,8 @@
       <c r="C31" s="10">
         <v>1</v>
       </c>
-      <c r="G31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -1140,12 +981,8 @@
       <c r="C32" s="10">
         <v>96</v>
       </c>
-      <c r="G32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -1155,12 +992,8 @@
       <c r="C33" s="10">
         <v>2838</v>
       </c>
-      <c r="G33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="9">
         <v>32</v>
       </c>
@@ -1170,15 +1003,8 @@
       <c r="C34" s="10">
         <v>568</v>
       </c>
-      <c r="F34" s="3">
-        <v>1676</v>
-      </c>
-      <c r="G34" s="3">
-        <f t="shared" si="0"/>
-        <v>2.9507042253521125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="9">
         <v>36</v>
       </c>
@@ -1189,7 +1015,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="9">
         <v>50</v>
       </c>
@@ -1200,7 +1026,7 @@
         <v>4478</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="9">
         <v>51</v>
       </c>
@@ -1211,7 +1037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="9">
         <v>52</v>
       </c>
@@ -1222,7 +1048,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="9">
         <v>53</v>
       </c>
@@ -1233,7 +1059,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="9">
         <v>55</v>
       </c>
@@ -1244,7 +1070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" s="9">
         <v>62</v>
       </c>
@@ -1253,46 +1079,6 @@
       </c>
       <c r="C41" s="10">
         <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="G43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="5">
-        <f>SUM(C5:C41)</f>
-        <v>623552</v>
-      </c>
-      <c r="F44" s="3">
-        <f>SUM(F5:F41)</f>
-        <v>586492</v>
-      </c>
-      <c r="G44" s="3">
-        <f>SUMIF(F5:F41,"&lt;&gt;",C5:C41)</f>
-        <v>319398</v>
-      </c>
-      <c r="H44" s="3">
-        <f>SUMIF(F5:F41,"",C5:C41)</f>
-        <v>304154</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G46" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G47" s="5">
-        <f>C30+C21</f>
-        <v>172566</v>
       </c>
     </row>
   </sheetData>
@@ -1301,32 +1087,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="19.149999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.25" style="3"/>
     <col min="2" max="3" width="19.875" style="3" customWidth="1"/>
     <col min="4" max="16384" width="11.25" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1"/>
+    <row r="4" spans="1:3" ht="19.149999999999999" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1337,7 +1123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="19.149999999999999" customHeight="1">
       <c r="A5" s="2">
         <v>2020</v>
       </c>
@@ -1348,7 +1134,7 @@
         <v>61625374.949999996</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="19.149999999999999" customHeight="1">
       <c r="A6" s="2">
         <v>2021</v>
       </c>
@@ -1359,7 +1145,7 @@
         <v>67067092.420000009</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="19.149999999999999" customHeight="1">
       <c r="A7" s="2">
         <v>2022</v>
       </c>
@@ -1370,7 +1156,7 @@
         <v>72838442.240000024</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="19.149999999999999" customHeight="1">
       <c r="A8" s="2">
         <v>2023</v>
       </c>
@@ -1381,7 +1167,7 @@
         <v>79235735.299999982</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="19.149999999999999" customHeight="1">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
     </row>

</xml_diff>